<commit_message>
Update TrainingData.xlsx with new data
</commit_message>
<xml_diff>
--- a/TrainingData.xlsx
+++ b/TrainingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob_barkai\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\hvss-calculator-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E5C49B-AF25-4F85-BDC8-DA5D2D36B5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E92A2B7-ED7B-46CC-AA38-97BF237ADC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="689" firstSheet="1" activeTab="1" xr2:uid="{511E2FD4-D8A9-4A5E-82F8-260385F23B95}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="689" firstSheet="1" activeTab="2" xr2:uid="{511E2FD4-D8A9-4A5E-82F8-260385F23B95}"/>
   </bookViews>
   <sheets>
     <sheet name="Use Cases" sheetId="42" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <definedName name="__extendedAttackComplexities">#REF!</definedName>
     <definedName name="__privilegesRequired">#REF!</definedName>
     <definedName name="__userInteractions">#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Input!$A$1:$T$220</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Input!$A$1:$T$209</definedName>
     <definedName name="Attack_Vector__AV____Network">#REF!</definedName>
     <definedName name="Extended_Attack_Complexity__EAC____Negligible">#REF!</definedName>
     <definedName name="Input">Input!$A$1:$T$182</definedName>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2339" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2519" uniqueCount="249">
   <si>
     <t>Case ID</t>
   </si>
@@ -1683,18 +1683,6 @@
     <xf numFmtId="0" fontId="6" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
@@ -1724,6 +1712,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3649,8 +3649,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{06F7F48A-5981-479B-9379-B03B0EF8229B}" name="Table151720" displayName="Table151720" ref="A1:E192" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92" tableBorderDxfId="91">
-  <autoFilter ref="A1:E192" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{06F7F48A-5981-479B-9379-B03B0EF8229B}" name="Table151720" displayName="Table151720" ref="A1:E210" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92" tableBorderDxfId="91">
+  <autoFilter ref="A1:E210" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}"/>
   <tableColumns count="5">
     <tableColumn id="2" xr3:uid="{C70DB743-1086-4C58-99BE-35A40D41E6DE}" name="AV" dataDxfId="90">
       <calculatedColumnFormula>MATCH(Input!B2, AV[Name],0)</calculatedColumnFormula>
@@ -3673,8 +3673,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F6E77A0E-B42B-4D44-9750-5A78CBD034AB}" name="Table1517" displayName="Table1517" ref="A1:H192" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" tableBorderDxfId="83">
-  <autoFilter ref="A1:H192" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F6E77A0E-B42B-4D44-9750-5A78CBD034AB}" name="Table1517" displayName="Table1517" ref="A1:H210" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" tableBorderDxfId="83">
+  <autoFilter ref="A1:H210" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}"/>
   <tableColumns count="8">
     <tableColumn id="2" xr3:uid="{936D37D9-DBF6-44CB-9065-1B33A762B0A9}" name="AV" dataDxfId="82">
       <calculatedColumnFormula>MATCH(Input!B2, AV[Name],0)</calculatedColumnFormula>
@@ -3706,8 +3706,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{642B3662-76CB-4C75-B48B-F02FD6640C33}" name="Table1518" displayName="Table1518" ref="A1:F192" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
-  <autoFilter ref="A1:F192" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{642B3662-76CB-4C75-B48B-F02FD6640C33}" name="Table1518" displayName="Table1518" ref="A1:F210" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
+  <autoFilter ref="A1:F210" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}"/>
   <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{55E9D0D1-0F05-4C10-8E71-999F2FBA7F98}" name="AV" dataDxfId="71">
       <calculatedColumnFormula>MATCH(Input!B2, AV[Name],0)</calculatedColumnFormula>
@@ -3733,8 +3733,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{42BD6C76-4116-4766-B5A4-D06567CB0786}" name="Table1519" displayName="Table1519" ref="A1:F192" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
-  <autoFilter ref="A1:F192" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{42BD6C76-4116-4766-B5A4-D06567CB0786}" name="Table1519" displayName="Table1519" ref="A1:F210" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
+  <autoFilter ref="A1:F210" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}"/>
   <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{A2A42F8F-191C-437A-B52A-067BDA09984A}" name="AV" dataDxfId="62">
       <calculatedColumnFormula>MATCH(Input!B2, AV[Name],0)</calculatedColumnFormula>
@@ -3760,8 +3760,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}" name="Table15" displayName="Table15" ref="A1:F192" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
-  <autoFilter ref="A1:F192" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}" name="Table15" displayName="Table15" ref="A1:F210" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
+  <autoFilter ref="A1:F210" xr:uid="{1CD8809F-B7CE-422F-B7CD-53FAAC74A134}"/>
   <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{58FC2918-72A4-4A6C-AB43-91D243882305}" name="AV" dataDxfId="53">
       <calculatedColumnFormula>MATCH(Input!B2, AV[Name],0)</calculatedColumnFormula>
@@ -5684,10 +5684,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="86"/>
+      <c r="B1" s="96"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
@@ -5753,10 +5753,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4849485A-0D09-495A-BE62-BD5587DADD9F}">
-  <dimension ref="A1:F192"/>
+  <dimension ref="A1:F210"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F192" sqref="F192"/>
+    <sheetView topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A209" sqref="A209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10756,15 +10756,483 @@
         <v>0.4</v>
       </c>
     </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="3">
+        <f>MATCH(Input!B193, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B193" s="3">
+        <f>MATCH(Input!C193, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C193" s="3">
+        <f>MATCH(Input!D193,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D193" s="3">
+        <f>MATCH(Input!E193, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E193" s="3">
+        <f>MATCH(Input!O193,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F193" s="35">
+        <f>Input!T193</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="3">
+        <f>MATCH(Input!B194, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B194" s="3">
+        <f>MATCH(Input!C194, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C194" s="3">
+        <f>MATCH(Input!D194,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D194" s="3">
+        <f>MATCH(Input!E194, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E194" s="3">
+        <f>MATCH(Input!O194,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F194" s="35">
+        <f>Input!T194</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="3">
+        <f>MATCH(Input!B195, AV[Name],0)</f>
+        <v>3</v>
+      </c>
+      <c r="B195" s="3">
+        <f>MATCH(Input!C195, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C195" s="3">
+        <f>MATCH(Input!D195,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D195" s="3">
+        <f>MATCH(Input!E195, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E195" s="3">
+        <f>MATCH(Input!O195,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F195" s="35">
+        <f>Input!T195</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="3">
+        <f>MATCH(Input!B196, AV[Name],0)</f>
+        <v>4</v>
+      </c>
+      <c r="B196" s="3">
+        <f>MATCH(Input!C196, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C196" s="3">
+        <f>MATCH(Input!D196,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D196" s="3">
+        <f>MATCH(Input!E196, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E196" s="3">
+        <f>MATCH(Input!O196,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F196" s="35">
+        <f>Input!T196</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="10">
+        <f>MATCH(Input!B197, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B197" s="10">
+        <f>MATCH(Input!C197, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C197" s="10">
+        <f>MATCH(Input!D197,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D197" s="10">
+        <f>MATCH(Input!E197, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E197" s="10">
+        <f>MATCH(Input!O197,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F197" s="36">
+        <f>Input!T197</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="3">
+        <f>MATCH(Input!B198, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B198" s="3">
+        <f>MATCH(Input!C198, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C198" s="3">
+        <f>MATCH(Input!D198,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D198" s="3">
+        <f>MATCH(Input!E198, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E198" s="3">
+        <f>MATCH(Input!O198,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F198" s="36">
+        <f>Input!T198</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="3">
+        <f>MATCH(Input!B199, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B199" s="3">
+        <f>MATCH(Input!C199, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C199" s="3">
+        <f>MATCH(Input!D199,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D199" s="3">
+        <f>MATCH(Input!E199, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E199" s="3">
+        <f>MATCH(Input!O199,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F199" s="36">
+        <f>Input!T199</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="3">
+        <f>MATCH(Input!B200, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B200" s="3">
+        <f>MATCH(Input!C200, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C200" s="3">
+        <f>MATCH(Input!D200,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D200" s="3">
+        <f>MATCH(Input!E200, UI[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="E200" s="3">
+        <f>MATCH(Input!O200,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F200" s="36">
+        <f>Input!T200</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="3">
+        <f>MATCH(Input!B201, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B201" s="3">
+        <f>MATCH(Input!C201, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C201" s="3">
+        <f>MATCH(Input!D201,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D201" s="3">
+        <f>MATCH(Input!E201, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E201" s="3">
+        <f>MATCH(Input!O201,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F201" s="36">
+        <f>Input!T201</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" s="3">
+        <f>MATCH(Input!B202, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B202" s="3">
+        <f>MATCH(Input!C202, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C202" s="3">
+        <f>MATCH(Input!D202,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D202" s="3">
+        <f>MATCH(Input!E202, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E202" s="3">
+        <f>MATCH(Input!O202,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F202" s="36">
+        <f>Input!T202</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" s="3">
+        <f>MATCH(Input!B203, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B203" s="3">
+        <f>MATCH(Input!C203, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C203" s="3">
+        <f>MATCH(Input!D203,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D203" s="3">
+        <f>MATCH(Input!E203, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E203" s="3">
+        <f>MATCH(Input!O203,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F203" s="35">
+        <f>Input!T203</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" s="3">
+        <f>MATCH(Input!B204, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B204" s="3">
+        <f>MATCH(Input!C204, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C204" s="3">
+        <f>MATCH(Input!D204,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D204" s="3">
+        <f>MATCH(Input!E204, UI[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="E204" s="3">
+        <f>MATCH(Input!O204,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F204" s="35">
+        <f>Input!T204</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" s="3">
+        <f>MATCH(Input!B205, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B205" s="3">
+        <f>MATCH(Input!C205, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C205" s="3">
+        <f>MATCH(Input!D205,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D205" s="3">
+        <f>MATCH(Input!E205, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E205" s="3">
+        <f>MATCH(Input!O205,XHB[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F205" s="35">
+        <f>Input!T205</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="3">
+        <f>MATCH(Input!B206, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B206" s="3">
+        <f>MATCH(Input!C206, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C206" s="3">
+        <f>MATCH(Input!D206,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D206" s="3">
+        <f>MATCH(Input!E206, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E206" s="3">
+        <f>MATCH(Input!O206,XHB[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F206" s="35">
+        <f>Input!T206</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" s="3">
+        <f>MATCH(Input!B207, AV[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="B207" s="3">
+        <f>MATCH(Input!C207, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C207" s="3">
+        <f>MATCH(Input!D207,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D207" s="3">
+        <f>MATCH(Input!E207, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E207" s="3">
+        <f>MATCH(Input!O207,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F207" s="36">
+        <f>Input!T207</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" s="3">
+        <f>MATCH(Input!B208, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B208" s="3">
+        <f>MATCH(Input!C208, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C208" s="3">
+        <f>MATCH(Input!D208,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D208" s="3">
+        <f>MATCH(Input!E208, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E208" s="3">
+        <f>MATCH(Input!O208,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F208" s="36">
+        <f>Input!T208</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="3">
+        <f>MATCH(Input!B209, AV[Name],0)</f>
+        <v>3</v>
+      </c>
+      <c r="B209" s="3">
+        <f>MATCH(Input!C209, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C209" s="3">
+        <f>MATCH(Input!D209,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D209" s="3">
+        <f>MATCH(Input!E209, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E209" s="3">
+        <f>MATCH(Input!O209,XHB[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F209" s="35">
+        <f>Input!T209</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="3">
+        <f>MATCH(Input!B210, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B210" s="3">
+        <f>MATCH(Input!C210, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C210" s="3">
+        <f>MATCH(Input!D210,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D210" s="3">
+        <f>MATCH(Input!E210, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E210" s="3">
+        <f>MATCH(Input!O210,XHB[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F210" s="35">
+        <f>Input!T210</f>
+        <v>2.7</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="User Interaction" prompt="Select the user interaction value from the list" sqref="D2:D192" xr:uid="{82B834EF-FA0E-42D2-8C27-901C66B25027}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" error="Please pick only a valid attack vector value from the list" sqref="A2:A192" xr:uid="{107A4EA4-ABD1-45A7-A94E-E06545E7455F}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="User Interaction" prompt="Select the user interaction value from the list" sqref="D2:D210" xr:uid="{82B834EF-FA0E-42D2-8C27-901C66B25027}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" error="Please pick only a valid attack vector value from the list" sqref="A2:A210" xr:uid="{107A4EA4-ABD1-45A7-A94E-E06545E7455F}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="UI" prompt="User Interaction" sqref="D1" xr:uid="{B8C3D384-0CEE-426A-8D14-4EB7DF743646}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="PR" prompt="Privilege Required" sqref="C1" xr:uid="{3C77F3B5-6E6A-4765-B016-845A263D877F}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="EAC" prompt="Attack Complexity" sqref="B1" xr:uid="{1CEE85BC-7C88-454E-A71C-6BE6DC7C35E9}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="AV" prompt="Attack Vector" sqref="A1" xr:uid="{3FFBD07A-F0AA-4DEA-85CF-D5797DE29151}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B2:C192 E2:E192" xr:uid="{6E2D2EEC-EB37-4078-B8E6-702D8DA5A389}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B2:C210 E2:E210" xr:uid="{6E2D2EEC-EB37-4078-B8E6-702D8DA5A389}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10788,10 +11256,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="86"/>
+      <c r="B1" s="96"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
@@ -11074,24 +11542,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="F1" s="88" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="F1" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="88"/>
-      <c r="I1" s="88" t="s">
+      <c r="G1" s="98"/>
+      <c r="I1" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="88"/>
-      <c r="L1" s="88" t="s">
+      <c r="J1" s="98"/>
+      <c r="L1" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="88"/>
+      <c r="M1" s="98"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -11647,10 +12115,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T192"/>
+  <dimension ref="A1:T210"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView topLeftCell="A185" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D214" sqref="D214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11676,22 +12144,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="92" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="92" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="93" t="s">
+      <c r="A1" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="89" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="38" t="s">
@@ -11703,22 +12171,22 @@
       <c r="I1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="94" t="s">
+      <c r="J1" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="95" t="s">
+      <c r="K1" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="96" t="s">
+      <c r="L1" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="97" t="s">
+      <c r="M1" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="98" t="s">
+      <c r="N1" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="99" t="s">
+      <c r="O1" s="95" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="85" t="s">
@@ -11753,7 +12221,7 @@
       <c r="E2" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="90">
+      <c r="F2" s="86">
         <v>5.0999999999999996</v>
       </c>
       <c r="G2" s="59" t="s">
@@ -24341,6 +24809,1194 @@
       </c>
       <c r="T192" s="71">
         <v>0.4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A193" s="40">
+        <v>192</v>
+      </c>
+      <c r="B193" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C193" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D193" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E193" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F193" s="72">
+        <v>7</v>
+      </c>
+      <c r="G193" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="H193" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="I193" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="J193" s="42" cm="1">
+        <f t="array" ref="J193">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G193) * (XCIA[Integrity]=Input!H193)*(XCIA[Availability]=Input!I193),0)), 1)</f>
+        <v>5.6</v>
+      </c>
+      <c r="K193" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L193" s="43">
+        <f>ROUND(VLOOKUP(K193,XPS[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="M193" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N193" s="44">
+        <f>ROUND(VLOOKUP(M193,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O193" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P193" s="49">
+        <f>ROUND(VLOOKUP(O193,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q193" s="71">
+        <v>3.8</v>
+      </c>
+      <c r="R193" s="71">
+        <v>0</v>
+      </c>
+      <c r="S193" s="71">
+        <v>0</v>
+      </c>
+      <c r="T193" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A194" s="40">
+        <v>193</v>
+      </c>
+      <c r="B194" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C194" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D194" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E194" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F194" s="72">
+        <v>6.5</v>
+      </c>
+      <c r="G194" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="H194" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="I194" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="J194" s="42" cm="1">
+        <f t="array" ref="J194">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G194) * (XCIA[Integrity]=Input!H194)*(XCIA[Availability]=Input!I194),0)), 1)</f>
+        <v>5.6</v>
+      </c>
+      <c r="K194" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L194" s="43">
+        <f>ROUND(VLOOKUP(K194,XPS[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="M194" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N194" s="44">
+        <f>ROUND(VLOOKUP(M194,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O194" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P194" s="49">
+        <f>ROUND(VLOOKUP(O194,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q194" s="71">
+        <v>3.8</v>
+      </c>
+      <c r="R194" s="71">
+        <v>0</v>
+      </c>
+      <c r="S194" s="71">
+        <v>0</v>
+      </c>
+      <c r="T194" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A195" s="40">
+        <v>194</v>
+      </c>
+      <c r="B195" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C195" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D195" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E195" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F195" s="72">
+        <v>5.2</v>
+      </c>
+      <c r="G195" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H195" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I195" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J195" s="42" cm="1">
+        <f t="array" ref="J195">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G195) * (XCIA[Integrity]=Input!H195)*(XCIA[Availability]=Input!I195),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K195" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L195" s="43">
+        <f>ROUND(VLOOKUP(K195,XPS[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="M195" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N195" s="44">
+        <f>ROUND(VLOOKUP(M195,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O195" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P195" s="49">
+        <f>ROUND(VLOOKUP(O195,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q195" s="71">
+        <v>0</v>
+      </c>
+      <c r="R195" s="71">
+        <v>1.6</v>
+      </c>
+      <c r="S195" s="71">
+        <v>0</v>
+      </c>
+      <c r="T195" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A196" s="40">
+        <v>195</v>
+      </c>
+      <c r="B196" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C196" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D196" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E196" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F196" s="72">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G196" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H196" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I196" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J196" s="42" cm="1">
+        <f t="array" ref="J196">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G196) * (XCIA[Integrity]=Input!H196)*(XCIA[Availability]=Input!I196),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K196" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L196" s="43">
+        <f>ROUND(VLOOKUP(K196,XPS[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="M196" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N196" s="44">
+        <f>ROUND(VLOOKUP(M196,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O196" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P196" s="49">
+        <f>ROUND(VLOOKUP(O196,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q196" s="71">
+        <v>0</v>
+      </c>
+      <c r="R196" s="71">
+        <v>1.5</v>
+      </c>
+      <c r="S196" s="71">
+        <v>0</v>
+      </c>
+      <c r="T196" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A197" s="40">
+        <v>196</v>
+      </c>
+      <c r="B197" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C197" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D197" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E197" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F197" s="72">
+        <v>7</v>
+      </c>
+      <c r="G197" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H197" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I197" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J197" s="42" cm="1">
+        <f t="array" ref="J197">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G197) * (XCIA[Integrity]=Input!H197)*(XCIA[Availability]=Input!I197),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K197" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L197" s="43">
+        <f>ROUND(VLOOKUP(K197,XPS[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="M197" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N197" s="44">
+        <f>ROUND(VLOOKUP(M197,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O197" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P197" s="49">
+        <f>ROUND(VLOOKUP(O197,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q197" s="71">
+        <v>0</v>
+      </c>
+      <c r="R197" s="71">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S197" s="71">
+        <v>0</v>
+      </c>
+      <c r="T197" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A198" s="40">
+        <v>197</v>
+      </c>
+      <c r="B198" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C198" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D198" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E198" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F198" s="72">
+        <v>6.5</v>
+      </c>
+      <c r="G198" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H198" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I198" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J198" s="42" cm="1">
+        <f t="array" ref="J198">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G198) * (XCIA[Integrity]=Input!H198)*(XCIA[Availability]=Input!I198),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K198" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L198" s="43">
+        <f>ROUND(VLOOKUP(K198,XPS[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="M198" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N198" s="44">
+        <f>ROUND(VLOOKUP(M198,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O198" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P198" s="49">
+        <f>ROUND(VLOOKUP(O198,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q198" s="71">
+        <v>0</v>
+      </c>
+      <c r="R198" s="71">
+        <v>2</v>
+      </c>
+      <c r="S198" s="71">
+        <v>0</v>
+      </c>
+      <c r="T198" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A199" s="40">
+        <v>198</v>
+      </c>
+      <c r="B199" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C199" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D199" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E199" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F199" s="72">
+        <v>6.5</v>
+      </c>
+      <c r="G199" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H199" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I199" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J199" s="42" cm="1">
+        <f t="array" ref="J199">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G199) * (XCIA[Integrity]=Input!H199)*(XCIA[Availability]=Input!I199),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K199" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L199" s="43">
+        <f>ROUND(VLOOKUP(K199,XPS[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="M199" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N199" s="44">
+        <f>ROUND(VLOOKUP(M199,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O199" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P199" s="49">
+        <f>ROUND(VLOOKUP(O199,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q199" s="71">
+        <v>0</v>
+      </c>
+      <c r="R199" s="71">
+        <v>2.1</v>
+      </c>
+      <c r="S199" s="71">
+        <v>0</v>
+      </c>
+      <c r="T199" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A200" s="40">
+        <v>199</v>
+      </c>
+      <c r="B200" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C200" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D200" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E200" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F200" s="72">
+        <v>6.3</v>
+      </c>
+      <c r="G200" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H200" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I200" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J200" s="42" cm="1">
+        <f t="array" ref="J200">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G200) * (XCIA[Integrity]=Input!H200)*(XCIA[Availability]=Input!I200),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K200" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L200" s="43">
+        <f>ROUND(VLOOKUP(K200,XPS[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="M200" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N200" s="44">
+        <f>ROUND(VLOOKUP(M200,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O200" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P200" s="49">
+        <f>ROUND(VLOOKUP(O200,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q200" s="71">
+        <v>0</v>
+      </c>
+      <c r="R200" s="71">
+        <v>1.9</v>
+      </c>
+      <c r="S200" s="71">
+        <v>0</v>
+      </c>
+      <c r="T200" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A201" s="40">
+        <v>200</v>
+      </c>
+      <c r="B201" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C201" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D201" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E201" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F201" s="72">
+        <v>7</v>
+      </c>
+      <c r="G201" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H201" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I201" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J201" s="42" cm="1">
+        <f t="array" ref="J201">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G201) * (XCIA[Integrity]=Input!H201)*(XCIA[Availability]=Input!I201),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K201" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L201" s="43">
+        <f>ROUND(VLOOKUP(K201,XPS[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="M201" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="N201" s="44">
+        <f>ROUND(VLOOKUP(M201,XSD[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="O201" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P201" s="49">
+        <f>ROUND(VLOOKUP(O201,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q201" s="71">
+        <v>0</v>
+      </c>
+      <c r="R201" s="71">
+        <v>0</v>
+      </c>
+      <c r="S201" s="71">
+        <v>2.5</v>
+      </c>
+      <c r="T201" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A202" s="40">
+        <v>201</v>
+      </c>
+      <c r="B202" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C202" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D202" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E202" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F202" s="72">
+        <v>6.5</v>
+      </c>
+      <c r="G202" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H202" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I202" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J202" s="42" cm="1">
+        <f t="array" ref="J202">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G202) * (XCIA[Integrity]=Input!H202)*(XCIA[Availability]=Input!I202),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K202" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L202" s="43">
+        <f>ROUND(VLOOKUP(K202,XPS[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="M202" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="N202" s="44">
+        <f>ROUND(VLOOKUP(M202,XSD[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="O202" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P202" s="49">
+        <f>ROUND(VLOOKUP(O202,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q202" s="71">
+        <v>0</v>
+      </c>
+      <c r="R202" s="71">
+        <v>0</v>
+      </c>
+      <c r="S202" s="71">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T202" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A203" s="40">
+        <v>202</v>
+      </c>
+      <c r="B203" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C203" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D203" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E203" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F203" s="72">
+        <v>6.5</v>
+      </c>
+      <c r="G203" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H203" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I203" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J203" s="42" cm="1">
+        <f t="array" ref="J203">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G203) * (XCIA[Integrity]=Input!H203)*(XCIA[Availability]=Input!I203),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K203" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L203" s="43">
+        <f>ROUND(VLOOKUP(K203,XPS[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="M203" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="N203" s="44">
+        <f>ROUND(VLOOKUP(M203,XSD[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="O203" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P203" s="49">
+        <f>ROUND(VLOOKUP(O203,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q203" s="71">
+        <v>0</v>
+      </c>
+      <c r="R203" s="71">
+        <v>0</v>
+      </c>
+      <c r="S203" s="71">
+        <v>2.4</v>
+      </c>
+      <c r="T203" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A204" s="40">
+        <v>203</v>
+      </c>
+      <c r="B204" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C204" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D204" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E204" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F204" s="72">
+        <v>6.3</v>
+      </c>
+      <c r="G204" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H204" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I204" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J204" s="42" cm="1">
+        <f t="array" ref="J204">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G204) * (XCIA[Integrity]=Input!H204)*(XCIA[Availability]=Input!I204),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K204" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L204" s="43">
+        <f>ROUND(VLOOKUP(K204,XPS[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="M204" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="N204" s="44">
+        <f>ROUND(VLOOKUP(M204,XSD[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="O204" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P204" s="49">
+        <f>ROUND(VLOOKUP(O204,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q204" s="71">
+        <v>0</v>
+      </c>
+      <c r="R204" s="71">
+        <v>0</v>
+      </c>
+      <c r="S204" s="71">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T204" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A205" s="40">
+        <v>204</v>
+      </c>
+      <c r="B205" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C205" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D205" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E205" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F205" s="72">
+        <v>7</v>
+      </c>
+      <c r="G205" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H205" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I205" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J205" s="42" cm="1">
+        <f t="array" ref="J205">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G205) * (XCIA[Integrity]=Input!H205)*(XCIA[Availability]=Input!I205),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K205" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L205" s="43">
+        <f>ROUND(VLOOKUP(K205,XPS[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="M205" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N205" s="44">
+        <f>ROUND(VLOOKUP(M205,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O205" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="P205" s="49">
+        <f>ROUND(VLOOKUP(O205,XHB[], 2, FALSE), 1)</f>
+        <v>7.5</v>
+      </c>
+      <c r="Q205" s="71">
+        <v>0</v>
+      </c>
+      <c r="R205" s="71">
+        <v>0</v>
+      </c>
+      <c r="S205" s="71">
+        <v>0</v>
+      </c>
+      <c r="T205" s="71">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="206" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A206" s="40">
+        <v>205</v>
+      </c>
+      <c r="B206" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C206" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D206" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E206" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F206" s="72">
+        <v>6.5</v>
+      </c>
+      <c r="G206" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H206" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I206" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J206" s="42" cm="1">
+        <f t="array" ref="J206">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G206) * (XCIA[Integrity]=Input!H206)*(XCIA[Availability]=Input!I206),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K206" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L206" s="43">
+        <f>ROUND(VLOOKUP(K206,XPS[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="M206" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N206" s="44">
+        <f>ROUND(VLOOKUP(M206,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O206" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="P206" s="49">
+        <f>ROUND(VLOOKUP(O206,XHB[], 2, FALSE), 1)</f>
+        <v>7.5</v>
+      </c>
+      <c r="Q206" s="71">
+        <v>0</v>
+      </c>
+      <c r="R206" s="71">
+        <v>0</v>
+      </c>
+      <c r="S206" s="71">
+        <v>0</v>
+      </c>
+      <c r="T206" s="71">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A207" s="40">
+        <v>206</v>
+      </c>
+      <c r="B207" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C207" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D207" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E207" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F207" s="72">
+        <v>6.9</v>
+      </c>
+      <c r="G207" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H207" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I207" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J207" s="42" cm="1">
+        <f t="array" ref="J207">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G207) * (XCIA[Integrity]=Input!H207)*(XCIA[Availability]=Input!I207),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K207" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L207" s="43">
+        <f>ROUND(VLOOKUP(K207,XPS[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="M207" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N207" s="44">
+        <f>ROUND(VLOOKUP(M207,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O207" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P207" s="49">
+        <f>ROUND(VLOOKUP(O207,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q207" s="71">
+        <v>0</v>
+      </c>
+      <c r="R207" s="71">
+        <v>2</v>
+      </c>
+      <c r="S207" s="71">
+        <v>0</v>
+      </c>
+      <c r="T207" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A208" s="40">
+        <v>207</v>
+      </c>
+      <c r="B208" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C208" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D208" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E208" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F208" s="72">
+        <v>6.5</v>
+      </c>
+      <c r="G208" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H208" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I208" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J208" s="42" cm="1">
+        <f t="array" ref="J208">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G208) * (XCIA[Integrity]=Input!H208)*(XCIA[Availability]=Input!I208),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K208" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L208" s="43">
+        <f>ROUND(VLOOKUP(K208,XPS[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="M208" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N208" s="44">
+        <f>ROUND(VLOOKUP(M208,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O208" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P208" s="49">
+        <f>ROUND(VLOOKUP(O208,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q208" s="71">
+        <v>0</v>
+      </c>
+      <c r="R208" s="71">
+        <v>1.9</v>
+      </c>
+      <c r="S208" s="71">
+        <v>0</v>
+      </c>
+      <c r="T208" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A209" s="40">
+        <v>208</v>
+      </c>
+      <c r="B209" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C209" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D209" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E209" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F209" s="72">
+        <v>5.2</v>
+      </c>
+      <c r="G209" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H209" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I209" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J209" s="42" cm="1">
+        <f t="array" ref="J209">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G209) * (XCIA[Integrity]=Input!H209)*(XCIA[Availability]=Input!I209),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K209" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L209" s="43">
+        <f>ROUND(VLOOKUP(K209,XPS[], 2, FALSE), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="M209" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N209" s="44">
+        <f>ROUND(VLOOKUP(M209,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O209" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P209" s="49">
+        <f>ROUND(VLOOKUP(O209,XHB[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q209" s="71">
+        <v>0</v>
+      </c>
+      <c r="R209" s="71">
+        <v>1.8</v>
+      </c>
+      <c r="S209" s="71">
+        <v>0</v>
+      </c>
+      <c r="T209" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A210" s="40">
+        <v>209</v>
+      </c>
+      <c r="B210" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C210" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D210" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E210" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F210" s="72">
+        <v>7</v>
+      </c>
+      <c r="G210" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H210" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I210" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J210" s="42" cm="1">
+        <f t="array" ref="J210">ROUND(INDEX(XCIA[Value], MATCH(1, (XCIA[Confidentiality]=Input!G210) * (XCIA[Integrity]=Input!H210)*(XCIA[Availability]=Input!I210),0)), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K210" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="L210" s="43">
+        <f>ROUND(VLOOKUP(K210,XPS[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="M210" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N210" s="44">
+        <f>ROUND(VLOOKUP(M210,XSD[], 2, FALSE), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O210" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="P210" s="49">
+        <f>ROUND(VLOOKUP(O210,XHB[], 2, FALSE), 1)</f>
+        <v>7.5</v>
+      </c>
+      <c r="Q210" s="71">
+        <v>0</v>
+      </c>
+      <c r="R210" s="71">
+        <v>0</v>
+      </c>
+      <c r="S210" s="71">
+        <v>0</v>
+      </c>
+      <c r="T210" s="71">
+        <v>2.7</v>
       </c>
     </row>
   </sheetData>
@@ -24352,15 +26008,15 @@
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="PR" prompt="Privilege Required" sqref="D1" xr:uid="{0689ECCC-AE3E-44D0-9FD7-28DCBE682106}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="EAC" prompt="Attack Complexity" sqref="C1" xr:uid="{4BAA72E6-A4B7-47B3-AE03-B6CCFACCAE9A}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="AV" prompt="Attack Vector" sqref="B1" xr:uid="{4125D245-588B-44ED-A120-3B9501B05E2E}"/>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="Score Validation" error="Score must be a number, and range between 0 and 10 (inclusive)" sqref="L2:L191 N2:N191 J2:J191 L192 N192 J192" xr:uid="{E28F2A3F-2D08-4469-BCFF-D471BB869B80}">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="Score Validation" error="Score must be a number, and range between 0 and 10 (inclusive)" sqref="L2:L210 J2:J210 N2:N210" xr:uid="{E28F2A3F-2D08-4469-BCFF-D471BB869B80}">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Score Validation" error="Score must be a number, and range between 0.1 and 10 (inclusive)" sqref="F2:F191 F192" xr:uid="{E0DE361F-98DE-4236-A40F-285DE7DC88F3}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Score Validation" error="Score must be a number, and range between 0.1 and 10 (inclusive)" sqref="F2:F210" xr:uid="{E0DE361F-98DE-4236-A40F-285DE7DC88F3}">
       <formula1>0.1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Score Validation" error="Score must be a number, and range between 0 and 10 (inclusive)" sqref="P2:P192 Q2:T192" xr:uid="{F7668674-C89A-46DE-9E2A-B222400D6CD6}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Score Validation" error="Score must be a number, and range between 0 and 10 (inclusive)" sqref="P2:T210" xr:uid="{F7668674-C89A-46DE-9E2A-B222400D6CD6}">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
@@ -24374,61 +26030,61 @@
           <x14:formula1>
             <xm:f>'Exploitability Metrics'!$G$3:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E191 E192</xm:sqref>
+          <xm:sqref>E2:E210</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Privileges Required (PR)" prompt="Select the privileges required value from the list" xr:uid="{463BA7FD-1F05-4E97-9E60-54876D73DFD2}">
           <x14:formula1>
             <xm:f>'Exploitability Metrics'!$E$3:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D191 D192</xm:sqref>
+          <xm:sqref>D2:D210</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Attack Complexity (EAC)" prompt="Select the attack complexity value from the list" xr:uid="{1A68C1C5-18CB-4D3B-8C86-A0D0A2A7AB38}">
           <x14:formula1>
             <xm:f>'Exploitability Metrics'!$C$3:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C191 C192</xm:sqref>
+          <xm:sqref>C2:C210</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please pick only a valid attack vector value from the list" promptTitle="Attack Vector (AV)" prompt="Select the attack vector value from the list" xr:uid="{CBCA14FF-AB72-4CD3-A3A0-F520ED0D3BD2}">
           <x14:formula1>
             <xm:f>'Exploitability Metrics'!$A$3:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B191 B192</xm:sqref>
+          <xm:sqref>B2:B210</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Patient Safety" prompt="Select the patient safety value from the list" xr:uid="{029DA38C-1B7B-4E45-A25D-6724FAF590E3}">
           <x14:formula1>
             <xm:f>'Impact Metrics'!$F$3:$F$7</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K191 K192</xm:sqref>
+          <xm:sqref>K2:K210</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sensitive Data" prompt="Select the sensitive data value from the list" xr:uid="{B7BFABEF-E8BE-43E0-84A9-0C135E97F99D}">
           <x14:formula1>
             <xm:f>'Impact Metrics'!$I$3:$I$7</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M191 M192</xm:sqref>
+          <xm:sqref>M2:M210</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hospital Breach" prompt="Select the hospital breach value from the list" xr:uid="{443B9126-FA23-4879-ABA4-5B9890875360}">
           <x14:formula1>
             <xm:f>'Impact Metrics'!$L$3:$L$6</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O192</xm:sqref>
+          <xm:sqref>O2:O210</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Confidentiality" prompt="Select the confidentiality value from the list" xr:uid="{D8348950-441C-4B0C-82E1-EC2200D5E3A3}">
           <x14:formula1>
             <xm:f>'Impact Metrics'!$A$34:$A$36</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G192</xm:sqref>
+          <xm:sqref>G2:G210</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Integrity" prompt="Select the integrity value from the list" xr:uid="{7A4C9296-81E0-4ABC-974E-B7CF746DA819}">
           <x14:formula1>
             <xm:f>'Impact Metrics'!$A$34:$A$36</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H192</xm:sqref>
+          <xm:sqref>H2:H210</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Availability" prompt="Select the availability value from the list" xr:uid="{0466EAA3-3E91-49BE-A7FD-7744245DA963}">
           <x14:formula1>
             <xm:f>'Impact Metrics'!$A$34:$A$36</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I192</xm:sqref>
+          <xm:sqref>I2:I210</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -24438,10 +26094,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACB9B37-E53A-4F8D-ADC2-B522F2F5EF8D}">
-  <dimension ref="A1:E192"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E192" sqref="E192"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G204" sqref="G204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28673,15 +30329,411 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="31">
+        <f>MATCH(Input!B193, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B193" s="31">
+        <f>MATCH(Input!C193, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C193" s="31">
+        <f>MATCH(Input!D193,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D193" s="31">
+        <f>MATCH(Input!E193, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E193" s="32">
+        <f>Input!F193</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="31">
+        <f>MATCH(Input!B194, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B194" s="31">
+        <f>MATCH(Input!C194, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C194" s="31">
+        <f>MATCH(Input!D194,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D194" s="31">
+        <f>MATCH(Input!E194, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E194" s="32">
+        <f>Input!F194</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="31">
+        <f>MATCH(Input!B195, AV[Name],0)</f>
+        <v>3</v>
+      </c>
+      <c r="B195" s="31">
+        <f>MATCH(Input!C195, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C195" s="31">
+        <f>MATCH(Input!D195,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D195" s="31">
+        <f>MATCH(Input!E195, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E195" s="32">
+        <f>Input!F195</f>
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="31">
+        <f>MATCH(Input!B196, AV[Name],0)</f>
+        <v>4</v>
+      </c>
+      <c r="B196" s="31">
+        <f>MATCH(Input!C196, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C196" s="31">
+        <f>MATCH(Input!D196,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D196" s="31">
+        <f>MATCH(Input!E196, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E196" s="32">
+        <f>Input!F196</f>
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="31">
+        <f>MATCH(Input!B197, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B197" s="31">
+        <f>MATCH(Input!C197, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C197" s="31">
+        <f>MATCH(Input!D197,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D197" s="31">
+        <f>MATCH(Input!E197, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E197" s="32">
+        <f>Input!F197</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="31">
+        <f>MATCH(Input!B198, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B198" s="31">
+        <f>MATCH(Input!C198, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C198" s="31">
+        <f>MATCH(Input!D198,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D198" s="31">
+        <f>MATCH(Input!E198, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E198" s="32">
+        <f>Input!F198</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="31">
+        <f>MATCH(Input!B199, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B199" s="31">
+        <f>MATCH(Input!C199, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C199" s="31">
+        <f>MATCH(Input!D199,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D199" s="31">
+        <f>MATCH(Input!E199, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E199" s="32">
+        <f>Input!F199</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="31">
+        <f>MATCH(Input!B200, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B200" s="31">
+        <f>MATCH(Input!C200, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C200" s="31">
+        <f>MATCH(Input!D200,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D200" s="31">
+        <f>MATCH(Input!E200, UI[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="E200" s="32">
+        <f>Input!F200</f>
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="31">
+        <f>MATCH(Input!B201, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B201" s="31">
+        <f>MATCH(Input!C201, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C201" s="31">
+        <f>MATCH(Input!D201,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D201" s="31">
+        <f>MATCH(Input!E201, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E201" s="32">
+        <f>Input!F201</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="31">
+        <f>MATCH(Input!B202, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B202" s="31">
+        <f>MATCH(Input!C202, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C202" s="31">
+        <f>MATCH(Input!D202,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D202" s="31">
+        <f>MATCH(Input!E202, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E202" s="32">
+        <f>Input!F202</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="31">
+        <f>MATCH(Input!B203, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B203" s="31">
+        <f>MATCH(Input!C203, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C203" s="31">
+        <f>MATCH(Input!D203,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D203" s="31">
+        <f>MATCH(Input!E203, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E203" s="32">
+        <f>Input!F203</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="31">
+        <f>MATCH(Input!B204, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B204" s="31">
+        <f>MATCH(Input!C204, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C204" s="31">
+        <f>MATCH(Input!D204,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D204" s="31">
+        <f>MATCH(Input!E204, UI[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="E204" s="32">
+        <f>Input!F204</f>
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="31">
+        <f>MATCH(Input!B205, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B205" s="31">
+        <f>MATCH(Input!C205, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C205" s="31">
+        <f>MATCH(Input!D205,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D205" s="31">
+        <f>MATCH(Input!E205, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E205" s="32">
+        <f>Input!F205</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="31">
+        <f>MATCH(Input!B206, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B206" s="31">
+        <f>MATCH(Input!C206, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C206" s="31">
+        <f>MATCH(Input!D206,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D206" s="31">
+        <f>MATCH(Input!E206, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E206" s="32">
+        <f>Input!F206</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="31">
+        <f>MATCH(Input!B207, AV[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="B207" s="31">
+        <f>MATCH(Input!C207, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C207" s="31">
+        <f>MATCH(Input!D207,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D207" s="31">
+        <f>MATCH(Input!E207, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E207" s="32">
+        <f>Input!F207</f>
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="31">
+        <f>MATCH(Input!B208, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B208" s="31">
+        <f>MATCH(Input!C208, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C208" s="31">
+        <f>MATCH(Input!D208,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D208" s="31">
+        <f>MATCH(Input!E208, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E208" s="32">
+        <f>Input!F208</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="31">
+        <f>MATCH(Input!B209, AV[Name],0)</f>
+        <v>3</v>
+      </c>
+      <c r="B209" s="31">
+        <f>MATCH(Input!C209, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C209" s="31">
+        <f>MATCH(Input!D209,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D209" s="31">
+        <f>MATCH(Input!E209, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E209" s="32">
+        <f>Input!F209</f>
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="31">
+        <f>MATCH(Input!B210, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B210" s="31">
+        <f>MATCH(Input!C210, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C210" s="31">
+        <f>MATCH(Input!D210,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D210" s="31">
+        <f>MATCH(Input!E210, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E210" s="32">
+        <f>Input!F210</f>
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="User Interaction" prompt="Select the user interaction value from the list" sqref="D2:D192" xr:uid="{FF0CB111-14FA-432F-A44A-3D33A169B47B}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" error="Please pick only a valid attack vector value from the list" sqref="A2:A192" xr:uid="{6A172E8D-36AB-4BFC-AF5E-F8F58C342BFF}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="User Interaction" prompt="Select the user interaction value from the list" sqref="D2:D210" xr:uid="{FF0CB111-14FA-432F-A44A-3D33A169B47B}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" error="Please pick only a valid attack vector value from the list" sqref="A2:A210" xr:uid="{6A172E8D-36AB-4BFC-AF5E-F8F58C342BFF}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="UI" prompt="User Interaction" sqref="D1" xr:uid="{82516B36-9114-435B-AA82-6F2F6A357B4D}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="PR" prompt="Privilege Required" sqref="C1" xr:uid="{EA79D6ED-5BD0-420B-9DF1-22DA06783E27}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="EAC" prompt="Attack Complexity" sqref="B1" xr:uid="{7DE74F70-CEDC-412A-A530-7AED80F0EEE2}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="AV" prompt="Attack Vector" sqref="A1" xr:uid="{5775941F-E8E2-4338-B376-8313D0C35DB0}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B2:C192" xr:uid="{9B022CE2-C20F-48AD-BE54-FBB4625943DB}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B2:C210" xr:uid="{9B022CE2-C20F-48AD-BE54-FBB4625943DB}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -28702,22 +30754,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="86"/>
-      <c r="D1" s="87" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="87"/>
-      <c r="G1" s="86" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="86"/>
-      <c r="J1" s="86" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="86"/>
+      <c r="A1" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="D1" s="97" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="97"/>
+      <c r="G1" s="96" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="96"/>
+      <c r="J1" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="96"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
@@ -28859,10 +30911,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCDD67B-6D21-4D18-A32F-D662679FA12D}">
-  <dimension ref="A1:H192"/>
+  <dimension ref="A1:H210"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A177" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J205" sqref="J205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35398,15 +37450,627 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A193" s="31">
+        <f>MATCH(Input!B193, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B193" s="31">
+        <f>MATCH(Input!C193, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C193" s="31">
+        <f>MATCH(Input!D193,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D193" s="31">
+        <f>MATCH(Input!E193, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E193" s="73">
+        <f>MATCH(Input!G193,XCIA_Values[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F193" s="74">
+        <f>MATCH(Input!H193,XCIA_Values[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="G193" s="74">
+        <f>MATCH(Input!I193,XCIA_Values[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="H193" s="26">
+        <f>Input!Q193</f>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A194" s="31">
+        <f>MATCH(Input!B194, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B194" s="31">
+        <f>MATCH(Input!C194, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C194" s="31">
+        <f>MATCH(Input!D194,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D194" s="31">
+        <f>MATCH(Input!E194, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E194" s="73">
+        <f>MATCH(Input!G194,XCIA_Values[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F194" s="74">
+        <f>MATCH(Input!H194,XCIA_Values[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="G194" s="74">
+        <f>MATCH(Input!I194,XCIA_Values[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="H194" s="32">
+        <f>Input!Q194</f>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A195" s="31">
+        <f>MATCH(Input!B195, AV[Name],0)</f>
+        <v>3</v>
+      </c>
+      <c r="B195" s="31">
+        <f>MATCH(Input!C195, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C195" s="31">
+        <f>MATCH(Input!D195,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D195" s="31">
+        <f>MATCH(Input!E195, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E195" s="75">
+        <f>MATCH(Input!G195,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F195" s="76">
+        <f>MATCH(Input!H195,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G195" s="76">
+        <f>MATCH(Input!I195,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H195" s="32">
+        <f>Input!Q195</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A196" s="31">
+        <f>MATCH(Input!B196, AV[Name],0)</f>
+        <v>4</v>
+      </c>
+      <c r="B196" s="31">
+        <f>MATCH(Input!C196, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C196" s="31">
+        <f>MATCH(Input!D196,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D196" s="31">
+        <f>MATCH(Input!E196, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E196" s="75">
+        <f>MATCH(Input!G196,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F196" s="76">
+        <f>MATCH(Input!H196,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G196" s="76">
+        <f>MATCH(Input!I196,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H196" s="32">
+        <f>Input!Q196</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A197" s="31">
+        <f>MATCH(Input!B197, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B197" s="31">
+        <f>MATCH(Input!C197, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C197" s="31">
+        <f>MATCH(Input!D197,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D197" s="31">
+        <f>MATCH(Input!E197, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E197" s="75">
+        <f>MATCH(Input!G197,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F197" s="76">
+        <f>MATCH(Input!H197,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G197" s="76">
+        <f>MATCH(Input!I197,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H197" s="32">
+        <f>Input!Q197</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A198" s="31">
+        <f>MATCH(Input!B198, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B198" s="31">
+        <f>MATCH(Input!C198, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C198" s="31">
+        <f>MATCH(Input!D198,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D198" s="31">
+        <f>MATCH(Input!E198, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E198" s="75">
+        <f>MATCH(Input!G198,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F198" s="76">
+        <f>MATCH(Input!H198,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G198" s="76">
+        <f>MATCH(Input!I198,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H198" s="32">
+        <f>Input!Q198</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A199" s="31">
+        <f>MATCH(Input!B199, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B199" s="31">
+        <f>MATCH(Input!C199, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C199" s="31">
+        <f>MATCH(Input!D199,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D199" s="31">
+        <f>MATCH(Input!E199, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E199" s="77">
+        <f>MATCH(Input!G199,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F199" s="78">
+        <f>MATCH(Input!H199,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G199" s="78">
+        <f>MATCH(Input!I199,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H199" s="32">
+        <f>Input!Q199</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A200" s="31">
+        <f>MATCH(Input!B200, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B200" s="31">
+        <f>MATCH(Input!C200, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C200" s="31">
+        <f>MATCH(Input!D200,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D200" s="31">
+        <f>MATCH(Input!E200, UI[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="E200" s="79">
+        <f>MATCH(Input!G200,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F200" s="80">
+        <f>MATCH(Input!H200,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G200" s="80">
+        <f>MATCH(Input!I200,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H200" s="32">
+        <f>Input!Q200</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A201" s="31">
+        <f>MATCH(Input!B201, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B201" s="31">
+        <f>MATCH(Input!C201, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C201" s="31">
+        <f>MATCH(Input!D201,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D201" s="31">
+        <f>MATCH(Input!E201, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E201" s="73">
+        <f>MATCH(Input!G201,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F201" s="74">
+        <f>MATCH(Input!H201,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G201" s="74">
+        <f>MATCH(Input!I201,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H201" s="26">
+        <f>Input!Q201</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A202" s="31">
+        <f>MATCH(Input!B202, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B202" s="31">
+        <f>MATCH(Input!C202, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C202" s="31">
+        <f>MATCH(Input!D202,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D202" s="31">
+        <f>MATCH(Input!E202, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E202" s="73">
+        <f>MATCH(Input!G202,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F202" s="74">
+        <f>MATCH(Input!H202,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G202" s="74">
+        <f>MATCH(Input!I202,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H202" s="32">
+        <f>Input!Q202</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A203" s="31">
+        <f>MATCH(Input!B203, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B203" s="31">
+        <f>MATCH(Input!C203, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C203" s="31">
+        <f>MATCH(Input!D203,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D203" s="31">
+        <f>MATCH(Input!E203, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E203" s="75">
+        <f>MATCH(Input!G203,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F203" s="76">
+        <f>MATCH(Input!H203,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G203" s="76">
+        <f>MATCH(Input!I203,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H203" s="32">
+        <f>Input!Q203</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A204" s="31">
+        <f>MATCH(Input!B204, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B204" s="31">
+        <f>MATCH(Input!C204, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C204" s="31">
+        <f>MATCH(Input!D204,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D204" s="31">
+        <f>MATCH(Input!E204, UI[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="E204" s="75">
+        <f>MATCH(Input!G204,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F204" s="76">
+        <f>MATCH(Input!H204,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G204" s="76">
+        <f>MATCH(Input!I204,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H204" s="32">
+        <f>Input!Q204</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A205" s="31">
+        <f>MATCH(Input!B205, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B205" s="31">
+        <f>MATCH(Input!C205, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C205" s="31">
+        <f>MATCH(Input!D205,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D205" s="31">
+        <f>MATCH(Input!E205, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E205" s="75">
+        <f>MATCH(Input!G205,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F205" s="76">
+        <f>MATCH(Input!H205,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G205" s="76">
+        <f>MATCH(Input!I205,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H205" s="32">
+        <f>Input!Q205</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A206" s="31">
+        <f>MATCH(Input!B206, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B206" s="31">
+        <f>MATCH(Input!C206, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C206" s="31">
+        <f>MATCH(Input!D206,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D206" s="31">
+        <f>MATCH(Input!E206, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E206" s="75">
+        <f>MATCH(Input!G206,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F206" s="76">
+        <f>MATCH(Input!H206,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G206" s="76">
+        <f>MATCH(Input!I206,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H206" s="32">
+        <f>Input!Q206</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207" s="31">
+        <f>MATCH(Input!B207, AV[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="B207" s="31">
+        <f>MATCH(Input!C207, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C207" s="31">
+        <f>MATCH(Input!D207,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D207" s="31">
+        <f>MATCH(Input!E207, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E207" s="73">
+        <f>MATCH(Input!G207,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F207" s="74">
+        <f>MATCH(Input!H207,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G207" s="74">
+        <f>MATCH(Input!I207,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H207" s="32">
+        <f>Input!Q207</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A208" s="31">
+        <f>MATCH(Input!B208, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B208" s="31">
+        <f>MATCH(Input!C208, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C208" s="31">
+        <f>MATCH(Input!D208,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D208" s="31">
+        <f>MATCH(Input!E208, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E208" s="75">
+        <f>MATCH(Input!G208,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F208" s="76">
+        <f>MATCH(Input!H208,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G208" s="76">
+        <f>MATCH(Input!I208,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H208" s="32">
+        <f>Input!Q208</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A209" s="31">
+        <f>MATCH(Input!B209, AV[Name],0)</f>
+        <v>3</v>
+      </c>
+      <c r="B209" s="31">
+        <f>MATCH(Input!C209, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C209" s="31">
+        <f>MATCH(Input!D209,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D209" s="31">
+        <f>MATCH(Input!E209, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E209" s="75">
+        <f>MATCH(Input!G209,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F209" s="76">
+        <f>MATCH(Input!H209,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G209" s="76">
+        <f>MATCH(Input!I209,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H209" s="32">
+        <f>Input!Q209</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A210" s="31">
+        <f>MATCH(Input!B210, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B210" s="31">
+        <f>MATCH(Input!C210, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C210" s="31">
+        <f>MATCH(Input!D210,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D210" s="31">
+        <f>MATCH(Input!E210, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E210" s="75">
+        <f>MATCH(Input!G210,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F210" s="76">
+        <f>MATCH(Input!H210,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G210" s="76">
+        <f>MATCH(Input!I210,XCIA_Values[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="H210" s="32">
+        <f>Input!Q210</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B2:C192 E2:G192" xr:uid="{7E275E2C-1054-412C-B52C-D29FE4EC545F}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B2:C210 E2:G210" xr:uid="{7E275E2C-1054-412C-B52C-D29FE4EC545F}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="AV" prompt="Attack Vector" sqref="A1" xr:uid="{D5018B4B-BFA2-4316-91BD-7E36BAD0B119}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="EAC" prompt="Attack Complexity" sqref="B1" xr:uid="{15B29146-71B0-4DB8-AD24-2EC959B37AA4}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="PR" prompt="Privilege Required" sqref="C1" xr:uid="{EB9FD5D0-736E-46DA-8864-37E0C537F6AF}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="UI" prompt="User Interaction" sqref="D1" xr:uid="{C71349C0-95C9-4EA8-B3D0-BBB2FACAB5EB}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" error="Please pick only a valid attack vector value from the list" sqref="A2:A192" xr:uid="{BF8D68F4-50DB-44D5-8581-28C050FBFA9D}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="User Interaction" prompt="Select the user interaction value from the list" sqref="D2:D192" xr:uid="{D1F7C618-F6E7-4D3E-8901-E14E24CCCC70}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" error="Please pick only a valid attack vector value from the list" sqref="A2:A210" xr:uid="{BF8D68F4-50DB-44D5-8581-28C050FBFA9D}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="User Interaction" prompt="Select the user interaction value from the list" sqref="D2:D210" xr:uid="{D1F7C618-F6E7-4D3E-8901-E14E24CCCC70}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -35427,18 +38091,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="D1" s="87" t="s">
+      <c r="B1" s="96"/>
+      <c r="D1" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="87"/>
-      <c r="G1" s="86" t="s">
+      <c r="E1" s="97"/>
+      <c r="G1" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="86"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
@@ -35533,10 +38197,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83AF5AF-BB2E-4F2A-A5F6-A91315A6D171}">
-  <dimension ref="A1:F192"/>
+  <dimension ref="A1:F210"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F192" sqref="F192"/>
+    <sheetView topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A198" sqref="A198:F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40536,15 +43200,483 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="3">
+        <f>MATCH(Input!B193, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B193" s="3">
+        <f>MATCH(Input!C193, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C193" s="3">
+        <f>MATCH(Input!D193,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D193" s="3">
+        <f>MATCH(Input!E193, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E193" s="3">
+        <f>MATCH(Input!K193,XPS[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F193" s="35">
+        <f>Input!R193</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="3">
+        <f>MATCH(Input!B194, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B194" s="3">
+        <f>MATCH(Input!C194, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C194" s="3">
+        <f>MATCH(Input!D194,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D194" s="3">
+        <f>MATCH(Input!E194, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E194" s="3">
+        <f>MATCH(Input!K194,XPS[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F194" s="35">
+        <f>Input!R194</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="3">
+        <f>MATCH(Input!B195, AV[Name],0)</f>
+        <v>3</v>
+      </c>
+      <c r="B195" s="3">
+        <f>MATCH(Input!C195, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C195" s="3">
+        <f>MATCH(Input!D195,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D195" s="3">
+        <f>MATCH(Input!E195, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E195" s="3">
+        <f>MATCH(Input!K195,XPS[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F195" s="35">
+        <f>Input!R195</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="3">
+        <f>MATCH(Input!B196, AV[Name],0)</f>
+        <v>4</v>
+      </c>
+      <c r="B196" s="3">
+        <f>MATCH(Input!C196, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C196" s="3">
+        <f>MATCH(Input!D196,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D196" s="3">
+        <f>MATCH(Input!E196, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E196" s="3">
+        <f>MATCH(Input!K196,XPS[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F196" s="35">
+        <f>Input!R196</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="3">
+        <f>MATCH(Input!B197, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B197" s="3">
+        <f>MATCH(Input!C197, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C197" s="3">
+        <f>MATCH(Input!D197,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D197" s="3">
+        <f>MATCH(Input!E197, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E197" s="3">
+        <f>MATCH(Input!K197,XPS[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F197" s="35">
+        <f>Input!R197</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="3">
+        <f>MATCH(Input!B198, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B198" s="3">
+        <f>MATCH(Input!C198, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C198" s="3">
+        <f>MATCH(Input!D198,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D198" s="3">
+        <f>MATCH(Input!E198, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E198" s="3">
+        <f>MATCH(Input!K198,XPS[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F198" s="35">
+        <f>Input!R198</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="10">
+        <f>MATCH(Input!B199, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B199" s="10">
+        <f>MATCH(Input!C199, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C199" s="10">
+        <f>MATCH(Input!D199,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D199" s="10">
+        <f>MATCH(Input!E199, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E199" s="10">
+        <f>MATCH(Input!K199,XPS[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F199" s="36">
+        <f>Input!R199</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="3">
+        <f>MATCH(Input!B200, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B200" s="3">
+        <f>MATCH(Input!C200, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C200" s="3">
+        <f>MATCH(Input!D200,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D200" s="3">
+        <f>MATCH(Input!E200, UI[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="E200" s="3">
+        <f>MATCH(Input!K200,XPS[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F200" s="36">
+        <f>Input!R200</f>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="3">
+        <f>MATCH(Input!B201, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B201" s="3">
+        <f>MATCH(Input!C201, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C201" s="3">
+        <f>MATCH(Input!D201,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D201" s="3">
+        <f>MATCH(Input!E201, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E201" s="3">
+        <f>MATCH(Input!K201,XPS[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F201" s="36">
+        <f>Input!R201</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" s="3">
+        <f>MATCH(Input!B202, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B202" s="3">
+        <f>MATCH(Input!C202, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C202" s="3">
+        <f>MATCH(Input!D202,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D202" s="3">
+        <f>MATCH(Input!E202, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E202" s="3">
+        <f>MATCH(Input!K202,XPS[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F202" s="36">
+        <f>Input!R202</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" s="3">
+        <f>MATCH(Input!B203, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B203" s="3">
+        <f>MATCH(Input!C203, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C203" s="3">
+        <f>MATCH(Input!D203,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D203" s="3">
+        <f>MATCH(Input!E203, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E203" s="3">
+        <f>MATCH(Input!K203,XPS[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F203" s="36">
+        <f>Input!R203</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" s="10">
+        <f>MATCH(Input!B204, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B204" s="10">
+        <f>MATCH(Input!C204, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C204" s="10">
+        <f>MATCH(Input!D204,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D204" s="10">
+        <f>MATCH(Input!E204, UI[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="E204" s="10">
+        <f>MATCH(Input!K204,XPS[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F204" s="36">
+        <f>Input!R204</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" s="10">
+        <f>MATCH(Input!B205, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B205" s="10">
+        <f>MATCH(Input!C205, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C205" s="10">
+        <f>MATCH(Input!D205,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D205" s="10">
+        <f>MATCH(Input!E205, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E205" s="10">
+        <f>MATCH(Input!K205,XPS[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F205" s="36">
+        <f>Input!R205</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="3">
+        <f>MATCH(Input!B206, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B206" s="3">
+        <f>MATCH(Input!C206, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C206" s="3">
+        <f>MATCH(Input!D206,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D206" s="3">
+        <f>MATCH(Input!E206, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E206" s="3">
+        <f>MATCH(Input!K206,XPS[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F206" s="35">
+        <f>Input!R206</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" s="3">
+        <f>MATCH(Input!B207, AV[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="B207" s="3">
+        <f>MATCH(Input!C207, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C207" s="3">
+        <f>MATCH(Input!D207,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D207" s="3">
+        <f>MATCH(Input!E207, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E207" s="3">
+        <f>MATCH(Input!K207,XPS[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F207" s="35">
+        <f>Input!R207</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" s="10">
+        <f>MATCH(Input!B208, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B208" s="10">
+        <f>MATCH(Input!C208, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C208" s="10">
+        <f>MATCH(Input!D208,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D208" s="10">
+        <f>MATCH(Input!E208, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E208" s="10">
+        <f>MATCH(Input!K208,XPS[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F208" s="36">
+        <f>Input!R208</f>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="3">
+        <f>MATCH(Input!B209, AV[Name],0)</f>
+        <v>3</v>
+      </c>
+      <c r="B209" s="3">
+        <f>MATCH(Input!C209, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C209" s="3">
+        <f>MATCH(Input!D209,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D209" s="3">
+        <f>MATCH(Input!E209, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E209" s="3">
+        <f>MATCH(Input!K209,XPS[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F209" s="36">
+        <f>Input!R209</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="3">
+        <f>MATCH(Input!B210, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B210" s="3">
+        <f>MATCH(Input!C210, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C210" s="3">
+        <f>MATCH(Input!D210,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D210" s="3">
+        <f>MATCH(Input!E210, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E210" s="3">
+        <f>MATCH(Input!K210,XPS[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F210" s="36">
+        <f>Input!R210</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B2:C192 E2:E192" xr:uid="{B116D84B-B277-4EB3-9A9F-562A76E8EC67}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B2:C210 E2:E210" xr:uid="{B116D84B-B277-4EB3-9A9F-562A76E8EC67}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="AV" prompt="Attack Vector" sqref="A1" xr:uid="{95544F25-4571-4F5E-B611-A5B753829DF0}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="EAC" prompt="Attack Complexity" sqref="B1" xr:uid="{81DA219E-26A3-43D1-9FA9-CBEA3308A828}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="PR" prompt="Privilege Required" sqref="C1" xr:uid="{7BD1AF7E-08F7-4210-9712-A6512ED2784B}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="UI" prompt="User Interaction" sqref="D1" xr:uid="{420A71FB-FE69-4558-8309-1CE96271169B}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" error="Please pick only a valid attack vector value from the list" sqref="A2:A192" xr:uid="{0E9DFDBB-8AEC-4D07-8ADC-96AC3B2CDB0B}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="User Interaction" prompt="Select the user interaction value from the list" sqref="D2:D192" xr:uid="{6EE26566-7A4A-41FB-BB6D-D354532A053C}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" error="Please pick only a valid attack vector value from the list" sqref="A2:A210" xr:uid="{0E9DFDBB-8AEC-4D07-8ADC-96AC3B2CDB0B}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="User Interaction" prompt="Select the user interaction value from the list" sqref="D2:D210" xr:uid="{6EE26566-7A4A-41FB-BB6D-D354532A053C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -40568,10 +43700,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="86"/>
+      <c r="B1" s="96"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
@@ -40637,10 +43769,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89BFBC12-B621-4D35-8D5E-75B00A7FED0E}">
-  <dimension ref="A1:F192"/>
+  <dimension ref="A1:F210"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F192" sqref="F192"/>
+    <sheetView topLeftCell="A181" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A198" sqref="A198:F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45640,15 +48772,483 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="3">
+        <f>MATCH(Input!B193, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B193" s="3">
+        <f>MATCH(Input!C193, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C193" s="3">
+        <f>MATCH(Input!D193,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D193" s="3">
+        <f>MATCH(Input!E193, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E193" s="3">
+        <f>MATCH(Input!M193,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F193" s="35">
+        <f>Input!S193</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="3">
+        <f>MATCH(Input!B194, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B194" s="3">
+        <f>MATCH(Input!C194, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C194" s="3">
+        <f>MATCH(Input!D194,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D194" s="3">
+        <f>MATCH(Input!E194, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E194" s="3">
+        <f>MATCH(Input!M194,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F194" s="35">
+        <f>Input!S194</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="3">
+        <f>MATCH(Input!B195, AV[Name],0)</f>
+        <v>3</v>
+      </c>
+      <c r="B195" s="3">
+        <f>MATCH(Input!C195, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C195" s="3">
+        <f>MATCH(Input!D195,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D195" s="3">
+        <f>MATCH(Input!E195, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E195" s="3">
+        <f>MATCH(Input!M195,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F195" s="35">
+        <f>Input!S195</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="10">
+        <f>MATCH(Input!B196, AV[Name],0)</f>
+        <v>4</v>
+      </c>
+      <c r="B196" s="10">
+        <f>MATCH(Input!C196, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C196" s="10">
+        <f>MATCH(Input!D196,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D196" s="10">
+        <f>MATCH(Input!E196, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E196" s="10">
+        <f>MATCH(Input!M196,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F196" s="36">
+        <f>Input!S196</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="3">
+        <f>MATCH(Input!B197, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B197" s="3">
+        <f>MATCH(Input!C197, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C197" s="3">
+        <f>MATCH(Input!D197,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D197" s="3">
+        <f>MATCH(Input!E197, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E197" s="3">
+        <f>MATCH(Input!M197,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F197" s="36">
+        <f>Input!S197</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="3">
+        <f>MATCH(Input!B198, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B198" s="3">
+        <f>MATCH(Input!C198, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C198" s="3">
+        <f>MATCH(Input!D198,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D198" s="3">
+        <f>MATCH(Input!E198, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E198" s="3">
+        <f>MATCH(Input!M198,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F198" s="36">
+        <f>Input!S198</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="3">
+        <f>MATCH(Input!B199, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B199" s="3">
+        <f>MATCH(Input!C199, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C199" s="3">
+        <f>MATCH(Input!D199,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D199" s="3">
+        <f>MATCH(Input!E199, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E199" s="3">
+        <f>MATCH(Input!M199,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F199" s="36">
+        <f>Input!S199</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="3">
+        <f>MATCH(Input!B200, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B200" s="3">
+        <f>MATCH(Input!C200, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C200" s="3">
+        <f>MATCH(Input!D200,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D200" s="3">
+        <f>MATCH(Input!E200, UI[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="E200" s="3">
+        <f>MATCH(Input!M200,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F200" s="36">
+        <f>Input!S200</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="3">
+        <f>MATCH(Input!B201, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B201" s="3">
+        <f>MATCH(Input!C201, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C201" s="3">
+        <f>MATCH(Input!D201,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D201" s="3">
+        <f>MATCH(Input!E201, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E201" s="3">
+        <f>MATCH(Input!M201,XSD[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F201" s="36">
+        <f>Input!S201</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" s="10">
+        <f>MATCH(Input!B202, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B202" s="10">
+        <f>MATCH(Input!C202, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C202" s="10">
+        <f>MATCH(Input!D202,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D202" s="10">
+        <f>MATCH(Input!E202, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E202" s="10">
+        <f>MATCH(Input!M202,XSD[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F202" s="36">
+        <f>Input!S202</f>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" s="3">
+        <f>MATCH(Input!B203, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B203" s="3">
+        <f>MATCH(Input!C203, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C203" s="3">
+        <f>MATCH(Input!D203,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D203" s="3">
+        <f>MATCH(Input!E203, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E203" s="3">
+        <f>MATCH(Input!M203,XSD[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F203" s="35">
+        <f>Input!S203</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" s="3">
+        <f>MATCH(Input!B204, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B204" s="3">
+        <f>MATCH(Input!C204, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C204" s="3">
+        <f>MATCH(Input!D204,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D204" s="3">
+        <f>MATCH(Input!E204, UI[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="E204" s="3">
+        <f>MATCH(Input!M204,XSD[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F204" s="35">
+        <f>Input!S204</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" s="3">
+        <f>MATCH(Input!B205, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B205" s="3">
+        <f>MATCH(Input!C205, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C205" s="3">
+        <f>MATCH(Input!D205,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D205" s="3">
+        <f>MATCH(Input!E205, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E205" s="3">
+        <f>MATCH(Input!M205,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F205" s="35">
+        <f>Input!S205</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="10">
+        <f>MATCH(Input!B206, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B206" s="10">
+        <f>MATCH(Input!C206, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C206" s="10">
+        <f>MATCH(Input!D206,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D206" s="10">
+        <f>MATCH(Input!E206, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E206" s="10">
+        <f>MATCH(Input!M206,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F206" s="36">
+        <f>Input!S206</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" s="3">
+        <f>MATCH(Input!B207, AV[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="B207" s="3">
+        <f>MATCH(Input!C207, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C207" s="3">
+        <f>MATCH(Input!D207,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D207" s="3">
+        <f>MATCH(Input!E207, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E207" s="3">
+        <f>MATCH(Input!M207,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F207" s="36">
+        <f>Input!S207</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" s="3">
+        <f>MATCH(Input!B208, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B208" s="3">
+        <f>MATCH(Input!C208, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C208" s="3">
+        <f>MATCH(Input!D208,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D208" s="3">
+        <f>MATCH(Input!E208, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E208" s="3">
+        <f>MATCH(Input!M208,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F208" s="36">
+        <f>Input!S208</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="3">
+        <f>MATCH(Input!B209, AV[Name],0)</f>
+        <v>3</v>
+      </c>
+      <c r="B209" s="3">
+        <f>MATCH(Input!C209, EAC[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="C209" s="3">
+        <f>MATCH(Input!D209,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D209" s="3">
+        <f>MATCH(Input!E209, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E209" s="3">
+        <f>MATCH(Input!M209,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F209" s="36">
+        <f>Input!S209</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="3">
+        <f>MATCH(Input!B210, AV[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="B210" s="3">
+        <f>MATCH(Input!C210, EAC[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="C210" s="3">
+        <f>MATCH(Input!D210,PR[Name],0)</f>
+        <v>2</v>
+      </c>
+      <c r="D210" s="3">
+        <f>MATCH(Input!E210, UI[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="E210" s="3">
+        <f>MATCH(Input!M210,XSD[Name],0)</f>
+        <v>1</v>
+      </c>
+      <c r="F210" s="36">
+        <f>Input!S210</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B2:C192 E2:E192" xr:uid="{6E6B4A10-81E2-4617-B9FF-7674818630DC}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B2:C210 E2:E210" xr:uid="{6E6B4A10-81E2-4617-B9FF-7674818630DC}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="AV" prompt="Attack Vector" sqref="A1" xr:uid="{4C2F5F21-2EE7-40DB-88F3-D2669266A058}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="EAC" prompt="Attack Complexity" sqref="B1" xr:uid="{D1F6AA38-2FE2-42A4-8A70-C06445529B19}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="PR" prompt="Privilege Required" sqref="C1" xr:uid="{B3FF8BCE-734C-4F3A-9703-ABB17CB833F8}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="UI" prompt="User Interaction" sqref="D1" xr:uid="{F3FC926F-D40A-40FC-9CD3-D57BF1A91502}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" error="Please pick only a valid attack vector value from the list" sqref="A2:A192" xr:uid="{21A288AC-A72A-46FC-8D97-88C76A1B3644}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="User Interaction" prompt="Select the user interaction value from the list" sqref="D2:D192" xr:uid="{6ACB7CFE-6323-45E8-A215-9C13DE8DEA76}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" error="Please pick only a valid attack vector value from the list" sqref="A2:A210" xr:uid="{21A288AC-A72A-46FC-8D97-88C76A1B3644}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="User Interaction" prompt="Select the user interaction value from the list" sqref="D2:D210" xr:uid="{6ACB7CFE-6323-45E8-A215-9C13DE8DEA76}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -45659,6 +49259,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9737d3a9-2335-4c07-b0b2-c288a40e3b20">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8730efe7-2fa2-4804-9755-7d04b0b198a4" xsi:nil="true"/>
+    <Observations xmlns="9737d3a9-2335-4c07-b0b2-c288a40e3b20" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010028D8A687481A9F488BB3F882504B6D71" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee3c27a5b23326cbdc722b44cf44e972">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9737d3a9-2335-4c07-b0b2-c288a40e3b20" xmlns:ns3="aaa18e45-0655-4974-9c56-32601d3204f4" xmlns:ns4="8730efe7-2fa2-4804-9755-7d04b0b198a4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bad92e66f903a961295a483f48fe2b97" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="9737d3a9-2335-4c07-b0b2-c288a40e3b20"/>
@@ -45914,28 +49535,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C8E2BA4-0CB4-4989-94F9-E9685B3A215B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="9737d3a9-2335-4c07-b0b2-c288a40e3b20"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="8730efe7-2fa2-4804-9755-7d04b0b198a4"/>
+    <ds:schemaRef ds:uri="aaa18e45-0655-4974-9c56-32601d3204f4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9737d3a9-2335-4c07-b0b2-c288a40e3b20">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8730efe7-2fa2-4804-9755-7d04b0b198a4" xsi:nil="true"/>
-    <Observations xmlns="9737d3a9-2335-4c07-b0b2-c288a40e3b20" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{184560D9-6802-4A11-92FF-6A30F62447FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06AD0D4F-B6B2-4A33-B0D7-C5FADC2B701C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -45954,30 +49580,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{184560D9-6802-4A11-92FF-6A30F62447FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C8E2BA4-0CB4-4989-94F9-E9685B3A215B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9737d3a9-2335-4c07-b0b2-c288a40e3b20"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="8730efe7-2fa2-4804-9755-7d04b0b198a4"/>
-    <ds:schemaRef ds:uri="aaa18e45-0655-4974-9c56-32601d3204f4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>